<commit_message>
Added missing transect lengths on Lake Florida
</commit_message>
<xml_diff>
--- a/Data/Season2/Transect datasheets (Responses).xlsx
+++ b/Data/Season2/Transect datasheets (Responses).xlsx
@@ -3153,6 +3153,9 @@
       <c r="H61" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I61" s="2">
+        <v>28.0</v>
+      </c>
       <c r="J61" s="2">
         <v>1.0</v>
       </c>
@@ -3197,6 +3200,9 @@
       <c r="H62" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I62" s="2">
+        <v>28.0</v>
+      </c>
       <c r="J62" s="2">
         <v>2.0</v>
       </c>
@@ -3241,6 +3247,9 @@
       <c r="H63" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I63" s="2">
+        <v>28.0</v>
+      </c>
       <c r="J63" s="2">
         <v>3.0</v>
       </c>
@@ -3285,6 +3294,9 @@
       <c r="H64" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I64" s="2">
+        <v>28.0</v>
+      </c>
       <c r="J64" s="2">
         <v>4.0</v>
       </c>
@@ -3329,6 +3341,9 @@
       <c r="H65" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I65" s="2">
+        <v>28.0</v>
+      </c>
       <c r="J65" s="2">
         <v>5.0</v>
       </c>
@@ -3373,6 +3388,9 @@
       <c r="H66" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I66" s="2">
+        <v>28.0</v>
+      </c>
       <c r="J66" s="2">
         <v>6.0</v>
       </c>
@@ -3417,6 +3435,9 @@
       <c r="H67" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I67" s="2">
+        <v>28.0</v>
+      </c>
       <c r="J67" s="2">
         <v>7.0</v>
       </c>
@@ -3460,6 +3481,9 @@
       </c>
       <c r="H68" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="I68" s="2">
+        <v>28.0</v>
       </c>
       <c r="J68" s="2">
         <v>8.0</v>

</xml_diff>